<commit_message>
more data fixes from last tranche.
</commit_message>
<xml_diff>
--- a/dashboard_loader/disability_labour_participation_uploader/disability_labour_participation.xlsx
+++ b/dashboard_loader/disability_labour_participation_uploader/disability_labour_participation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -135,7 +135,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">National Disability Strategy 2010-2020 Second Implementation Plan</t>
+      <t xml:space="preserve">National Disability Strategy 2010–2020 Second Implementation Plan</t>
     </r>
     <r>
       <rPr>
@@ -156,7 +156,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Driving Action 2015-2018</t>
+      <t xml:space="preserve">Driving Action 2015–2018</t>
     </r>
     <r>
       <rPr>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">Influences</t>
   </si>
   <si>
-    <t xml:space="preserve">Labour force participation is impacted by the severity and type of disability, and levels of participation are less for those with more than one type of impairment and for those who experience disability at older ages. Other factors include the state of the job market, workplace conditions and workplace discrimination (OECD, 2010).</t>
+    <t xml:space="preserve">Labour force participation is impacted by the severity and type of disability, and levels of participation are less for those with more than one type of impairment and for those who experience disability at older ages. Other factors include the state of the job market, workplace conditions and workplace discrimination (OECD 2010).</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -186,30 +186,48 @@
   </si>
   <si>
     <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABS Survey of Disability, Ageing and Carers, various years.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">References</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The Organisation for Economic Co-operation and Development (OECD), 2010, </t>
+      <t xml:space="preserve">ABS Survey of Disability, Ageing and Carers, various years</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; Steering Committee for the Review of Government Service Provision (SCRGSP) 2018, Report on Government Services 2018, table 15A.77.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">References</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The Organisation for Economic Co-operation and Development (OECD) 2010, </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Sickness, Disability and Work: Breaking the Barriers: A Synthesis of Findings across OECD Countries. </t>
@@ -224,7 +242,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -248,16 +266,22 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -270,72 +294,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <i val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -344,21 +302,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="1"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,74 +317,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -452,7 +345,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -476,190 +369,78 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -668,16 +449,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="8.57"/>
   </cols>
   <sheetData>
@@ -791,7 +572,7 @@
         <v>1.1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>2009</v>
       </c>
@@ -826,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>2009</v>
       </c>
@@ -845,7 +626,7 @@
         <v>59.8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>2009</v>
       </c>
@@ -864,7 +645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>2009</v>
       </c>
@@ -883,7 +664,7 @@
         <v>1.7063681659955</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>2009</v>
       </c>
@@ -902,7 +683,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>2009</v>
       </c>
@@ -913,7 +694,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>2009</v>
       </c>
@@ -924,7 +705,7 @@
         <v>1.77009579341941</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>2012</v>
       </c>
@@ -959,7 +740,7 @@
         <v>52.8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>2012</v>
       </c>
@@ -994,7 +775,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>2012</v>
       </c>
@@ -1029,7 +810,7 @@
         <v>1.23106060606061</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>2012</v>
       </c>
@@ -1037,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1048,7 +829,7 @@
         <v>56.6</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>2012</v>
       </c>
@@ -1067,7 +848,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>2012</v>
       </c>
@@ -1086,7 +867,7 @@
         <v>1.08170476671234</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>2012</v>
       </c>
@@ -1105,7 +886,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>2012</v>
       </c>
@@ -1124,7 +905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>2012</v>
       </c>
@@ -1143,7 +924,7 @@
         <v>2.08246563931695</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>2015</v>
       </c>
@@ -1248,7 +1029,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>2015</v>
       </c>
@@ -1267,7 +1048,7 @@
         <v>57.8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>2015</v>
       </c>
@@ -1282,11 +1063,12 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="3" t="n">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K25" s="6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="M25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>2015</v>
       </c>
@@ -1304,8 +1086,9 @@
       <c r="K26" s="3" t="n">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>2015</v>
       </c>
@@ -1323,8 +1106,9 @@
       <c r="K27" s="3" t="n">
         <v>49.4</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>2015</v>
       </c>
@@ -1339,11 +1123,12 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="3" t="n">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K28" s="6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>2015</v>
       </c>
@@ -1362,7 +1147,7 @@
         <v>2.2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>2018</v>
       </c>
@@ -1399,104 +1184,104 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="12" t="n">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="9" t="s">
+    <row r="7" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+      <c r="B7" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+    <row r="8" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="12" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>